<commit_message>
Suite assemblage + paramétrage
Pour l'instant, que la partie fixation godet
</commit_message>
<xml_diff>
--- a/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
+++ b/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\Cours\S8\ELC D-6 PLM Maquette numérique\3-Notre projet\PLM_S8_21\02-Assemblage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CE1F88-472B-4627-BFF6-675ADAD41E58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F40743B-E62A-4C16-A7D7-C337DFEA10F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6216" yWindow="1128" windowWidth="17580" windowHeight="11436" xr2:uid="{35AA728D-CCB6-4C16-BB83-0BC538D34D24}"/>
+    <workbookView xWindow="-16104" yWindow="1812" windowWidth="23040" windowHeight="12360" xr2:uid="{35AA728D-CCB6-4C16-BB83-0BC538D34D24}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Rayon_interieur_pneu (mm)</t>
   </si>
@@ -49,6 +49,93 @@
   </si>
   <si>
     <t>Hauteur_coussin_pneu (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_dent_godet (mm)</t>
+  </si>
+  <si>
+    <t>Largeur_dent_godet (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_dent_godet (mm)</t>
+  </si>
+  <si>
+    <t>Depassement_dent_godet (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_godet (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_courbure_godet (mm)</t>
+  </si>
+  <si>
+    <t>Angle_dattaque_godet (deg)</t>
+  </si>
+  <si>
+    <t>Epaisseur_godet (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_liaison_godet (mm)</t>
+  </si>
+  <si>
+    <t>Largeur_liaison_godet (mm)</t>
+  </si>
+  <si>
+    <t>Longeur_liaison_godet (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_liaison_godet (mm)</t>
+  </si>
+  <si>
+    <t>Largeur_godet (mm)</t>
+  </si>
+  <si>
+    <t>Grande_largeur_fixation (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_fixation (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_fixation_attache_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Largeur_fiaxation_attache_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longueur_barre_couplage (mm) </t>
+  </si>
+  <si>
+    <t>Epaisseur_barre_menante (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_ext_couplage_fixation (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_int_barre_menante (mm)</t>
+  </si>
+  <si>
+    <t>Largeur_barre_menantte (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_avant_bras_couplage (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_barre_menante (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_int_menante_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_ext_menant_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_ext_couplage_menante (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_menante (mm)</t>
   </si>
 </sst>
 </file>
@@ -72,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -80,12 +167,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,54 +500,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6231B640-F325-49FA-B57B-99FFE5CE8D61}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="39.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B1">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <f>B6/6</f>
+        <v>21.666666666666668</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>300</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>200</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <f>8/10*MIN(B17,B20*2)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <f>B18</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <f>B17/2+B16/2</f>
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <f>B26*1.3</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <f>B20*1.3</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B47">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Parametrage de toute la partie pelle
</commit_message>
<xml_diff>
--- a/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
+++ b/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\Cours\S8\ELC D-6 PLM Maquette numérique\3-Notre projet\PLM_S8_21\02-Assemblage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F40743B-E62A-4C16-A7D7-C337DFEA10F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05438920-F106-40F6-ADA1-FD8C718CA3AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16104" yWindow="1812" windowWidth="23040" windowHeight="12360" xr2:uid="{35AA728D-CCB6-4C16-BB83-0BC538D34D24}"/>
+    <workbookView xWindow="-17064" yWindow="1728" windowWidth="23040" windowHeight="12360" xr2:uid="{35AA728D-CCB6-4C16-BB83-0BC538D34D24}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,22 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
-  <si>
-    <t>Rayon_interieur_pneu (mm)</t>
-  </si>
-  <si>
-    <t>Epaisseur_pneu (mm)</t>
-  </si>
-  <si>
-    <t>Rayon_exterieur_pneu (mm)</t>
-  </si>
-  <si>
-    <t>Largeur_pneu (mm)</t>
-  </si>
-  <si>
-    <t>Hauteur_coussin_pneu (mm)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Longueur_dent_godet (mm)</t>
   </si>
@@ -136,6 +121,135 @@
   </si>
   <si>
     <t>Epaisseur_menante (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_verin_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Largeur_verin_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Largeur_tete_godet_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Hauteur_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Largeur_ext_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Grosse_largeur_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_attache_godet_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_attache_tete_godet_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_tete_godet_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>hauteur_barre_menante_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Largeur_barre_menante_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_barre_menante_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_ailettes_verin_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_verin_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_attache_bras_sur_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_verin_avant_bras_verin (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_tige_verin_avant_bras_verin (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_corps_verin_avant_bras_verin (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_rotule_verin_avant_bras_verin (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_tige_verin_avant_bras_verin (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_bras_bras (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_dattache_bras_chassis (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_verin_bras (mm)</t>
+  </si>
+  <si>
+    <t>Largeur_verin_bras (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_ailettes_verin_bras (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_verin_bras (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_dattache_bras_avant_bras (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_ext_avant_bras_bras (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_verin_chassis_bras (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_verin_avant_bras_bras (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_tige_verin_avant_bras_bras (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_tige_verin_avant_bras_bras_verin (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_corps_verin_avant_bras_bras_verin (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_rotule_verin_avant_bras_bras_verin (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_verin_bras_chassis (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_tige_verin_bras_chassis (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_tige_verin_bras_chassis (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_rotule_corps_verin_chassis (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_rotule_tige_verin_bras_chassis (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_corps_verin_bras_chassis (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_rotule_tige_bras_chassis (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_rotule_corps_bras_chassis (mm)</t>
   </si>
 </sst>
 </file>
@@ -500,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6231B640-F325-49FA-B57B-99FFE5CE8D61}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,7 +627,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>50</v>
@@ -521,7 +635,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <f>B6/6</f>
@@ -530,7 +644,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -538,7 +652,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -546,7 +660,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>270</v>
@@ -554,7 +668,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>130</v>
@@ -562,7 +676,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>125</v>
@@ -570,7 +684,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>66</v>
@@ -578,7 +692,7 @@
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>15</v>
@@ -586,7 +700,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>10</v>
@@ -594,7 +708,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>80</v>
@@ -602,7 +716,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>100</v>
@@ -610,7 +724,7 @@
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>86</v>
@@ -618,7 +732,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3">
         <v>210</v>
@@ -626,7 +740,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3">
         <v>110</v>
@@ -634,7 +748,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3">
         <v>45</v>
@@ -642,7 +756,7 @@
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B17" s="4">
         <v>50</v>
@@ -650,7 +764,7 @@
     </row>
     <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4">
         <v>100</v>
@@ -658,7 +772,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3">
         <v>180</v>
@@ -666,7 +780,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B20" s="3">
         <v>20</v>
@@ -674,7 +788,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <f>8/10*MIN(B17,B20*2)</f>
@@ -683,7 +797,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <f>B18</f>
@@ -692,7 +806,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <f>B17/2+B16/2</f>
@@ -701,7 +815,7 @@
     </row>
     <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2">
         <v>300</v>
@@ -709,7 +823,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>210</v>
@@ -717,7 +831,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>20</v>
@@ -725,7 +839,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <f>B26*1.3</f>
@@ -734,59 +848,384 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <f>B20*1.3</f>
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B29">
+      <c r="B34" s="3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <f>B17/2</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <f>B18</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <f>B26</f>
         <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>1</v>
+      <c r="A43" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="B43">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>0</v>
+      <c r="A44" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B44">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <f>B31/2*1.1</f>
+        <v>825.00000000000011</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47">
+        <f>B46*1.1</f>
+        <v>907.50000000000023</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2">
+        <f>B44*1.4</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51">
         <v>300</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>4</v>
-      </c>
-      <c r="B47">
-        <v>2</v>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <f>60</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <f>B44</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <f>B45</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <f>B57*3</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2">
+        <f>B56</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <f>B53*2/3</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <f>B60</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <f>B48</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1">
+        <f>B49</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="2">
+        <f>B50</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67">
+        <f>B52</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68">
+        <f>B59</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70">
+        <f>B62</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <f>1.3*B68</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="2">
+        <f>1.3*B67</f>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cohérence des dimensions du bras
et beaux vérins
</commit_message>
<xml_diff>
--- a/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
+++ b/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\Cours\S8\ELC D-6 PLM Maquette numérique\3-Notre projet\PLM_S8_21\02-Assemblage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35F9F41-1223-446D-AF6C-790C1FE0F77A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A312F529-5F67-46C6-B39A-0738A21710D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6264" yWindow="9240" windowWidth="23040" windowHeight="12360" xr2:uid="{35AA728D-CCB6-4C16-BB83-0BC538D34D24}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{35AA728D-CCB6-4C16-BB83-0BC538D34D24}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6231B640-F325-49FA-B57B-99FFE5CE8D61}">
   <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,7 +636,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -644,8 +644,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f>B6/6</f>
-        <v>21.666666666666668</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -653,7 +652,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -661,7 +660,8 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <f>B1*2/5</f>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -669,7 +669,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>270</v>
+        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -677,7 +677,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>130</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -685,7 +685,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>125</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -693,7 +693,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>66</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -701,7 +701,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -725,7 +725,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -733,7 +733,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -875,7 +875,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="3">
-        <v>2200</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -883,8 +883,8 @@
         <v>30</v>
       </c>
       <c r="B31" s="3">
-        <f>0.94*B30</f>
-        <v>2068</v>
+        <f>0.9*B30</f>
+        <v>1620</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -1008,7 +1008,7 @@
       </c>
       <c r="B46">
         <f>B31/2*1.1</f>
-        <v>1137.4000000000001</v>
+        <v>891.00000000000011</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B47">
         <f>B46*1.1</f>
-        <v>1251.1400000000001</v>
+        <v>980.10000000000025</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -1066,7 +1066,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>1500</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1074,7 +1074,7 @@
         <v>72</v>
       </c>
       <c r="B54">
-        <v>2020</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1082,7 +1082,7 @@
         <v>73</v>
       </c>
       <c r="B55">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1090,7 +1090,7 @@
         <v>53</v>
       </c>
       <c r="B56">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -1125,8 +1125,8 @@
         <v>57</v>
       </c>
       <c r="B60">
-        <f>B59*4</f>
-        <v>100</v>
+        <f>MAX(B53/15,B59*2)</f>
+        <v>133.33333333333334</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="B62">
         <f>B53*2/3</f>
-        <v>1000</v>
+        <v>1333.3333333333333</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B63">
         <f>B62</f>
-        <v>1000</v>
+        <v>1333.3333333333333</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -1188,7 +1188,8 @@
         <v>64</v>
       </c>
       <c r="B67">
-        <v>1500</v>
+        <f>B54*2/3</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -1196,7 +1197,8 @@
         <v>65</v>
       </c>
       <c r="B68">
-        <v>1600</v>
+        <f>B54*2/3</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fin paramétrage + problème pneu
</commit_message>
<xml_diff>
--- a/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
+++ b/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\Cours\S8\ELC D-6 PLM Maquette numérique\3-Notre projet\PLM_S8_21\02-Assemblage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexb\Documents\PLM_S8_21\02-Assemblage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D900EE93-C926-4E99-B66C-64C2E8C00120}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6D2A75-51C3-4316-ABBC-DFAAB0CB6E81}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{35AA728D-CCB6-4C16-BB83-0BC538D34D24}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{35AA728D-CCB6-4C16-BB83-0BC538D34D24}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>Longueur_dent_godet (mm)</t>
   </si>
@@ -343,6 +334,27 @@
   </si>
   <si>
     <t>Hauteur_plot_pneu (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_corps_verin_direction (mm)</t>
+  </si>
+  <si>
+    <t>Rayon_tige_verin_direction (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_tige_verin_direction (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_chape_pivot_direction (mm)</t>
+  </si>
+  <si>
+    <t>Longueur_verin_direction (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_chape_pivot_direction (mm)</t>
+  </si>
+  <si>
+    <t>Rayon rotule_pivot_direction_verin (mm)</t>
   </si>
 </sst>
 </file>
@@ -707,18 +719,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6231B640-F325-49FA-B57B-99FFE5CE8D61}">
-  <dimension ref="A1:B103"/>
+  <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="L110" sqref="L110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5546875" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -726,7 +738,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -734,7 +746,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -742,7 +754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -751,7 +763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -759,7 +771,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -767,7 +779,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -775,7 +787,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -783,7 +795,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -791,7 +803,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -799,7 +811,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -807,7 +819,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -815,7 +827,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -823,7 +835,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -831,7 +843,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -839,7 +851,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -848,7 +860,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
@@ -856,7 +868,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -864,7 +876,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -872,7 +884,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -881,7 +893,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -890,7 +902,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
@@ -899,7 +911,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -908,7 +920,7 @@
         <v>56.25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
@@ -916,7 +928,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -924,7 +936,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -932,7 +944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -940,7 +952,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -949,7 +961,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>28</v>
       </c>
@@ -957,7 +969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -965,7 +977,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -974,7 +986,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -982,7 +994,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
@@ -990,7 +1002,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
@@ -998,7 +1010,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
@@ -1006,7 +1018,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -1014,7 +1026,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -1023,7 +1035,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
@@ -1031,7 +1043,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
@@ -1040,7 +1052,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
@@ -1048,7 +1060,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
@@ -1056,7 +1068,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
@@ -1065,7 +1077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
@@ -1073,7 +1085,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
@@ -1081,7 +1093,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>44</v>
       </c>
@@ -1089,7 +1101,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
@@ -1098,7 +1110,7 @@
         <v>891.00000000000011</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>49</v>
       </c>
@@ -1107,7 +1119,7 @@
         <v>980.10000000000025</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>46</v>
       </c>
@@ -1115,7 +1127,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>47</v>
       </c>
@@ -1123,7 +1135,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>48</v>
       </c>
@@ -1132,7 +1144,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>50</v>
       </c>
@@ -1140,7 +1152,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
@@ -1149,7 +1161,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
@@ -1157,7 +1169,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>72</v>
       </c>
@@ -1165,7 +1177,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>73</v>
       </c>
@@ -1173,7 +1185,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>53</v>
       </c>
@@ -1181,7 +1193,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>54</v>
       </c>
@@ -1190,7 +1202,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>55</v>
       </c>
@@ -1199,7 +1211,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>56</v>
       </c>
@@ -1208,7 +1220,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
@@ -1217,7 +1229,7 @@
         <v>133.33333333333334</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>58</v>
       </c>
@@ -1226,7 +1238,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>59</v>
       </c>
@@ -1235,7 +1247,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>60</v>
       </c>
@@ -1244,7 +1256,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>61</v>
       </c>
@@ -1253,7 +1265,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>62</v>
       </c>
@@ -1262,7 +1274,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>63</v>
       </c>
@@ -1271,7 +1283,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>64</v>
       </c>
@@ -1280,7 +1292,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>65</v>
       </c>
@@ -1289,7 +1301,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>67</v>
       </c>
@@ -1298,7 +1310,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>68</v>
       </c>
@@ -1307,7 +1319,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>69</v>
       </c>
@@ -1316,7 +1328,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>66</v>
       </c>
@@ -1325,7 +1337,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>70</v>
       </c>
@@ -1334,7 +1346,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>71</v>
       </c>
@@ -1343,55 +1355,61 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B75">
-        <v>1510</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+        <f>1.15*B89</f>
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B76">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+        <f>B90*1.2</f>
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B77">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+        <f>B80</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B78">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+        <f>MAX(0.21*B77,100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B79">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+        <f>1/2*B75</f>
+        <v>632.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B80">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+        <f>1/2.5*B90</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>80</v>
       </c>
@@ -1399,7 +1417,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>81</v>
       </c>
@@ -1407,7 +1425,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>82</v>
       </c>
@@ -1415,7 +1433,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>83</v>
       </c>
@@ -1423,15 +1441,16 @@
         <v>400</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B85">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <f>1/20*B76</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>85</v>
       </c>
@@ -1439,15 +1458,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B87" s="3">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <f>B79</f>
+        <v>632.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>87</v>
       </c>
@@ -1455,48 +1475,50 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B89" s="3">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B90" s="3">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B91" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+        <f>B85</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B92" s="3">
         <f>0.6*B95+B96/4-B91</f>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+        <v>48.75</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B93" s="3">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <f>1.5*B102</f>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>93</v>
       </c>
@@ -1504,7 +1526,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>94</v>
       </c>
@@ -1512,16 +1534,16 @@
         <v>160</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>95</v>
       </c>
       <c r="B96" s="2">
         <f>B91/2</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>96</v>
       </c>
@@ -1529,7 +1551,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>97</v>
       </c>
@@ -1537,7 +1559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>98</v>
       </c>
@@ -1545,7 +1567,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>99</v>
       </c>
@@ -1553,7 +1575,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>100</v>
       </c>
@@ -1561,20 +1583,77 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B102" s="3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B104" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B105" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B106" s="3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107" s="3">
         <v>270</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B103" s="3">
-        <v>5</v>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B108" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B109" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <f>10/12*B94</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Résolution pblm verin direction
</commit_message>
<xml_diff>
--- a/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
+++ b/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexb\Documents\PLM_S8_21\02-Assemblage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\Cours\S8\ELC D-6 PLM Maquette numérique\3-Notre projet\PLM_S8_21\02-Assemblage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA410B4B-D6FC-4D33-99CC-E254F0C8F223}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83192B69-3CC8-48FD-AD97-9A6C519D1C3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{35AA728D-CCB6-4C16-BB83-0BC538D34D24}"/>
+    <workbookView xWindow="4404" yWindow="1140" windowWidth="16884" windowHeight="10704" xr2:uid="{35AA728D-CCB6-4C16-BB83-0BC538D34D24}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>Longueur_dent_godet (mm)</t>
   </si>
@@ -355,6 +364,9 @@
   </si>
   <si>
     <t>Rayon rotule_pivot_direction_verin (mm)</t>
+  </si>
+  <si>
+    <t>Epaisseur_rotule_pivot_direction (mm)</t>
   </si>
 </sst>
 </file>
@@ -719,18 +731,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6231B640-F325-49FA-B57B-99FFE5CE8D61}">
-  <dimension ref="A1:B110"/>
+  <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="H100" sqref="H100"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
+    <col min="1" max="1" width="39.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -738,7 +750,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -746,7 +758,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -754,7 +766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -763,7 +775,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -771,7 +783,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -779,7 +791,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -787,7 +799,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -795,7 +807,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -803,7 +815,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -811,7 +823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -819,7 +831,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -827,7 +839,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -835,7 +847,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -843,7 +855,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -851,7 +863,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -860,7 +872,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
@@ -868,7 +880,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -876,7 +888,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -884,7 +896,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -893,7 +905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -902,7 +914,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
@@ -911,7 +923,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -920,7 +932,7 @@
         <v>56.25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
@@ -928,7 +940,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -936,7 +948,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -944,7 +956,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -952,7 +964,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -961,7 +973,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>28</v>
       </c>
@@ -969,7 +981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -977,7 +989,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -986,7 +998,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
@@ -1002,7 +1014,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
@@ -1018,7 +1030,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -1026,7 +1038,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -1035,7 +1047,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
@@ -1043,7 +1055,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
@@ -1052,7 +1064,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
@@ -1060,7 +1072,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
@@ -1068,7 +1080,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
@@ -1077,7 +1089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
@@ -1085,7 +1097,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
@@ -1093,7 +1105,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>44</v>
       </c>
@@ -1101,7 +1113,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
@@ -1110,7 +1122,7 @@
         <v>891.00000000000011</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>49</v>
       </c>
@@ -1119,7 +1131,7 @@
         <v>980.10000000000025</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>46</v>
       </c>
@@ -1127,7 +1139,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>47</v>
       </c>
@@ -1135,7 +1147,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>48</v>
       </c>
@@ -1144,7 +1156,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>50</v>
       </c>
@@ -1152,7 +1164,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
@@ -1161,7 +1173,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
@@ -1169,7 +1181,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>72</v>
       </c>
@@ -1177,7 +1189,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>73</v>
       </c>
@@ -1185,7 +1197,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>53</v>
       </c>
@@ -1193,7 +1205,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>54</v>
       </c>
@@ -1202,7 +1214,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>55</v>
       </c>
@@ -1211,7 +1223,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>56</v>
       </c>
@@ -1220,7 +1232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
@@ -1229,7 +1241,7 @@
         <v>133.33333333333334</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>58</v>
       </c>
@@ -1238,7 +1250,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>59</v>
       </c>
@@ -1247,7 +1259,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>60</v>
       </c>
@@ -1256,7 +1268,7 @@
         <v>1333.3333333333333</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>61</v>
       </c>
@@ -1265,7 +1277,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>62</v>
       </c>
@@ -1274,7 +1286,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>63</v>
       </c>
@@ -1283,7 +1295,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>64</v>
       </c>
@@ -1292,7 +1304,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>65</v>
       </c>
@@ -1301,7 +1313,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>67</v>
       </c>
@@ -1310,7 +1322,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>68</v>
       </c>
@@ -1319,7 +1331,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>69</v>
       </c>
@@ -1328,7 +1340,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>66</v>
       </c>
@@ -1337,7 +1349,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>70</v>
       </c>
@@ -1346,7 +1358,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>71</v>
       </c>
@@ -1355,34 +1367,34 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B75">
         <f>1.15*B89</f>
-        <v>1265</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1494.9999999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B76">
         <f>B90*1.2</f>
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B77">
         <f>B80</f>
-        <v>360</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>78</v>
       </c>
@@ -1391,25 +1403,25 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B79">
         <f>1/2*B75</f>
-        <v>632.5</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>747.49999999999989</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B80">
         <f>1/2.5*B90</f>
-        <v>360</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>80</v>
       </c>
@@ -1417,7 +1429,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>81</v>
       </c>
@@ -1425,7 +1437,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>82</v>
       </c>
@@ -1433,7 +1445,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>83</v>
       </c>
@@ -1441,16 +1453,16 @@
         <v>400</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B85">
         <f>1/20*B76</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>85</v>
       </c>
@@ -1458,16 +1470,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B87" s="3">
         <f>B79</f>
-        <v>632.5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>747.49999999999989</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>87</v>
       </c>
@@ -1475,50 +1487,50 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B89" s="3">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B90" s="3">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B91" s="3">
         <f>B85</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B92" s="3">
         <f>0.6*B95+B96/4-B91</f>
-        <v>48.75</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B93" s="3">
-        <f>1.5*B102</f>
-        <v>345</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>1.1*B102</f>
+        <v>253.00000000000003</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
         <v>93</v>
       </c>
@@ -1526,7 +1538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>94</v>
       </c>
@@ -1534,16 +1546,16 @@
         <v>160</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
         <v>95</v>
       </c>
       <c r="B96" s="2">
         <f>B91/2</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>96</v>
       </c>
@@ -1551,7 +1563,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>97</v>
       </c>
@@ -1559,7 +1571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>98</v>
       </c>
@@ -1567,7 +1579,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>99</v>
       </c>
@@ -1575,7 +1587,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>100</v>
       </c>
@@ -1583,7 +1595,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>101</v>
       </c>
@@ -1591,7 +1603,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="4" t="s">
         <v>102</v>
       </c>
@@ -1599,7 +1611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>103</v>
       </c>
@@ -1607,7 +1619,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>104</v>
       </c>
@@ -1615,15 +1627,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B106" s="3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>107</v>
       </c>
@@ -1631,7 +1643,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>106</v>
       </c>
@@ -1639,7 +1651,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>108</v>
       </c>
@@ -1647,12 +1659,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B110">
         <f>10/12*B94</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B111">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nouvelle assemblage et tout fonctionne presque trop bien
On peut commencer la macro
</commit_message>
<xml_diff>
--- a/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
+++ b/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\Cours\S8\ELC D-6 PLM Maquette numérique\3-Notre projet\PLM_S8_21\02-Assemblage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83192B69-3CC8-48FD-AD97-9A6C519D1C3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1380BEC2-BF6B-4561-9E8D-B49050DC2D39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4404" yWindow="1140" windowWidth="16884" windowHeight="10704" xr2:uid="{35AA728D-CCB6-4C16-BB83-0BC538D34D24}"/>
   </bookViews>
@@ -731,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6231B640-F325-49FA-B57B-99FFE5CE8D61}">
-  <dimension ref="A1:B111"/>
+  <dimension ref="A1:B112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112:B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1508,8 +1508,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="3">
-        <f>B85</f>
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -1518,7 +1517,7 @@
       </c>
       <c r="B92" s="3">
         <f>0.6*B95+B96/4-B91</f>
-        <v>43.5</v>
+        <v>61</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -1552,7 +1551,7 @@
       </c>
       <c r="B96" s="2">
         <f>B91/2</f>
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -1632,7 +1631,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="3">
-        <v>280</v>
+        <v>200</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -1640,7 +1639,7 @@
         <v>107</v>
       </c>
       <c r="B107" s="3">
-        <v>270</v>
+        <v>180</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -1668,13 +1667,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="3" t="s">
+    <row r="111" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B111">
+      <c r="B111" s="2">
         <v>10</v>
       </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Début Macro by RCT
</commit_message>
<xml_diff>
--- a/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
+++ b/02-Assemblage/Parametrage_de_la_pelleteuse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Etudes\Centrale\Cours\S8\ELC D-6 PLM Maquette numérique\3-Notre projet\PLM_S8_21\02-Assemblage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1380BEC2-BF6B-4561-9E8D-B49050DC2D39}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A56E743-9431-487D-A350-8A3062CD1720}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4404" yWindow="1140" windowWidth="16884" windowHeight="10704" xr2:uid="{35AA728D-CCB6-4C16-BB83-0BC538D34D24}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{35AA728D-CCB6-4C16-BB83-0BC538D34D24}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -731,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6231B640-F325-49FA-B57B-99FFE5CE8D61}">
-  <dimension ref="A1:B112"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112:B112"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,31 +742,40 @@
     <col min="1" max="1" width="39.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -774,96 +783,133 @@
         <f>B1*2/5</f>
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <f>C1*2/5</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>600</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6">
         <v>450</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>200</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
         <v>150</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="3">
         <v>210</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="3">
         <v>110</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" s="3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -871,32 +917,45 @@
         <f>B37*2.5</f>
         <v>62.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C16" s="3">
+        <f>C37*2.5</f>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="4">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="3">
         <v>260</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -904,8 +963,12 @@
         <f>B44</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="3">
+        <f>C44</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -913,8 +976,12 @@
         <f>8/10*MIN(B17,B20*2)</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f>8/10*MIN(C17,C20*2)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>22</v>
       </c>
@@ -922,8 +989,12 @@
         <f>B18</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <f>C18</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
@@ -931,40 +1002,56 @@
         <f>B17/2+B16/2</f>
         <v>56.25</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <f>C17/2+C16/2</f>
+        <v>56.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="2">
         <v>300</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B25">
         <v>230</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B26">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B27">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -972,24 +1059,34 @@
         <f>40</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <f>40</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="3">
         <v>1800</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" s="3">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
@@ -997,48 +1094,67 @@
         <f>0.9*B30</f>
         <v>1620</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" s="3">
+        <f>0.9*C30</f>
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="3">
         <v>180</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" s="3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B33" s="3">
         <v>190</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" s="3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="3">
         <v>410</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" s="3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B35" s="3">
         <v>200</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B36" s="3">
         <v>210</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36" s="3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
@@ -1046,16 +1162,23 @@
         <f>B17/2</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <f>C17/2</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B38">
         <v>100</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>38</v>
       </c>
@@ -1063,24 +1186,34 @@
         <f>B18</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <f>C18</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B40">
         <v>80</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B41">
         <v>135</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>41</v>
       </c>
@@ -1088,32 +1221,45 @@
         <f>B26</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <f>C26</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B43">
         <v>45</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B44">
         <v>25</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C44">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B45" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
@@ -1121,8 +1267,12 @@
         <f>B31/2*1.1</f>
         <v>891.00000000000011</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <f>C31/2*1.1</f>
+        <v>891.00000000000011</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>49</v>
       </c>
@@ -1130,24 +1280,34 @@
         <f>B46*1.1</f>
         <v>980.10000000000025</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <f>C46*1.1</f>
+        <v>980.10000000000025</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B48">
         <v>35</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B49">
         <v>40</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C49">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>48</v>
       </c>
@@ -1155,16 +1315,23 @@
         <f>B44*1.4</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50" s="2">
+        <f>C44*1.4</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B51">
         <v>300</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>51</v>
       </c>
@@ -1172,40 +1339,56 @@
         <f>B81</f>
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <f>C81</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B53">
         <v>2000</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>72</v>
       </c>
       <c r="B54">
         <v>1500</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>73</v>
       </c>
       <c r="B55">
         <v>140</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B56">
         <v>150</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>54</v>
       </c>
@@ -1213,8 +1396,12 @@
         <f>60</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <f>60</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>55</v>
       </c>
@@ -1222,8 +1409,12 @@
         <f>B44</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <f>C44</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>56</v>
       </c>
@@ -1231,8 +1422,12 @@
         <f>B45</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <f>C45</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>57</v>
       </c>
@@ -1240,8 +1435,12 @@
         <f>MAX(B53/15,B59*2)</f>
         <v>133.33333333333334</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C60">
+        <f>MAX(C53/15,C59*2)</f>
+        <v>133.33333333333334</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>58</v>
       </c>
@@ -1249,8 +1448,12 @@
         <f>B58</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61" s="2">
+        <f>C58</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>59</v>
       </c>
@@ -1258,8 +1461,12 @@
         <f>B53*2/3</f>
         <v>1333.3333333333333</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <f>C53*2/3</f>
+        <v>1333.3333333333333</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>60</v>
       </c>
@@ -1267,8 +1474,12 @@
         <f>B62</f>
         <v>1333.3333333333333</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63">
+        <f>C62</f>
+        <v>1333.3333333333333</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>61</v>
       </c>
@@ -1276,8 +1487,12 @@
         <f>B48</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64">
+        <f>C48</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>62</v>
       </c>
@@ -1285,8 +1500,12 @@
         <f>B49</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C65" s="1">
+        <f>C49</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>63</v>
       </c>
@@ -1294,8 +1513,12 @@
         <f>B50</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66" s="2">
+        <f>C50</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>64</v>
       </c>
@@ -1303,8 +1526,12 @@
         <f>B54*2/3</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67">
+        <f>C54*2/3</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>65</v>
       </c>
@@ -1312,8 +1539,12 @@
         <f>B54*2/3</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68">
+        <f>C54*2/3</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>67</v>
       </c>
@@ -1321,8 +1552,12 @@
         <f>B82</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69">
+        <f>C82</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>68</v>
       </c>
@@ -1330,8 +1565,12 @@
         <f>B61</f>
         <v>25</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C70">
+        <f>C61</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>69</v>
       </c>
@@ -1339,8 +1578,12 @@
         <f>B65</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71">
+        <f>C65</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>66</v>
       </c>
@@ -1348,8 +1591,12 @@
         <f>B64</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72">
+        <f>C64</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>70</v>
       </c>
@@ -1357,8 +1604,12 @@
         <f>1.3*B70</f>
         <v>32.5</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C73">
+        <f>1.3*C70</f>
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>71</v>
       </c>
@@ -1366,8 +1617,12 @@
         <f>1.3*B69</f>
         <v>32.5</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74" s="2">
+        <f>1.3*C69</f>
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>74</v>
       </c>
@@ -1375,8 +1630,12 @@
         <f>1.15*B89</f>
         <v>1494.9999999999998</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C75">
+        <f>1.15*C89</f>
+        <v>1609.9999999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>77</v>
       </c>
@@ -1384,8 +1643,12 @@
         <f>B90*1.2</f>
         <v>1200</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76">
+        <f>C90*1.2</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>76</v>
       </c>
@@ -1393,8 +1656,12 @@
         <f>B80</f>
         <v>400</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C77">
+        <f>C80</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>78</v>
       </c>
@@ -1402,8 +1669,12 @@
         <f>MAX(0.21*B77,100)</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C78">
+        <f>MAX(0.21*C77,100)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>75</v>
       </c>
@@ -1411,8 +1682,12 @@
         <f>1/2*B75</f>
         <v>747.49999999999989</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C79">
+        <f>1/2*C75</f>
+        <v>804.99999999999989</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>79</v>
       </c>
@@ -1420,40 +1695,56 @@
         <f>1/2.5*B90</f>
         <v>400</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C80">
+        <f>1/2.5*C90</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B81">
         <v>50</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C81">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B82">
         <v>25</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C82">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B83">
         <v>450</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C83">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>83</v>
       </c>
       <c r="B84">
         <v>400</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C84">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>84</v>
       </c>
@@ -1461,16 +1752,23 @@
         <f>1/20*B76</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C85">
+        <f>1/20*C76</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B86" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C86" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>86</v>
       </c>
@@ -1478,40 +1776,56 @@
         <f>B79</f>
         <v>747.49999999999989</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C87" s="3">
+        <f>C79</f>
+        <v>804.99999999999989</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>87</v>
       </c>
       <c r="B88" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C88" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B89" s="3">
         <v>1300</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C89" s="3">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B90" s="3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C90" s="3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B91" s="3">
         <v>40</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C91" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>91</v>
       </c>
@@ -1519,8 +1833,12 @@
         <f>0.6*B95+B96/4-B91</f>
         <v>61</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C92" s="3">
+        <f>0.6*C95+C96/4-C91</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>92</v>
       </c>
@@ -1528,24 +1846,34 @@
         <f>1.1*B102</f>
         <v>253.00000000000003</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C93" s="3">
+        <f>1.1*C102</f>
+        <v>253.00000000000003</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
         <v>93</v>
       </c>
       <c r="B94" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C94" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B95" s="3">
         <v>160</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C95" s="3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
         <v>95</v>
       </c>
@@ -1553,112 +1881,155 @@
         <f>B91/2</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C96" s="2">
+        <f>C91/2</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B97" s="3">
         <v>175</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C97" s="3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B98" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C98" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B99" s="3">
         <v>200</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C99" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>99</v>
       </c>
       <c r="B100" s="4">
         <v>190</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C100" s="4">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B101" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C101" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B102" s="3">
         <v>230</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C102" s="3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B103" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C103" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>103</v>
       </c>
       <c r="B104" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C104" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B105" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C105" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B106" s="3">
         <v>200</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C106" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B107" s="3">
         <v>180</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C107" s="3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B108" s="3">
         <v>30</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C108" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B109" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C109" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>109</v>
       </c>
@@ -1666,16 +2037,23 @@
         <f>10/12*B94</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C110">
+        <f>10/12*C94</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
         <v>110</v>
       </c>
       <c r="B111" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C111" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="3"/>
     </row>
   </sheetData>

</xml_diff>